<commit_message>
Plugging in LWW/M777 dates.
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Greg Sanders\Documents\Development\JointDevelopment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Development\JointDevelopment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12210" windowHeight="7395"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11460"/>
   </bookViews>
   <sheets>
     <sheet name="Cost" sheetId="1" r:id="rId1"/>
     <sheet name="Schedule" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" calcMode="manual"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="42">
   <si>
     <t>Approved IOC</t>
   </si>
@@ -136,6 +136,21 @@
   </si>
   <si>
     <t>FY2019</t>
+  </si>
+  <si>
+    <t>Army LW155/M777</t>
+  </si>
+  <si>
+    <t>LW155_M777_Schedule_2003_12_8yearSequence.csv</t>
+  </si>
+  <si>
+    <t>USMC LW155/M777</t>
+  </si>
+  <si>
+    <t>LW155_M777_Schedule_2003_6_8yearSequence</t>
+  </si>
+  <si>
+    <t>LW155_M777_Schedule_2004_13_7yearSequence</t>
   </si>
 </sst>
 </file>
@@ -144,7 +159,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -189,7 +204,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -198,9 +213,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -230,7 +246,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>199386</xdr:colOff>
+      <xdr:colOff>132711</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>171188</xdr:rowOff>
     </xdr:to>
@@ -559,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +589,7 @@
     <col min="6" max="6" width="13.42578125" customWidth="1"/>
     <col min="7" max="7" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -640,7 +656,7 @@
         <v>37768</v>
       </c>
       <c r="E2" s="1">
-        <v>39845</v>
+        <v>39859</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" t="s">
@@ -665,7 +681,7 @@
         <v>22</v>
       </c>
       <c r="E3" s="5">
-        <v>42248</v>
+        <v>42262</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="4" t="s">
@@ -706,7 +722,7 @@
         <v>81.297976273551996</v>
       </c>
       <c r="I4" s="1">
-        <v>37165</v>
+        <v>37179</v>
       </c>
       <c r="N4">
         <f>R4*1000/P4</f>
@@ -751,7 +767,7 @@
         <v>161.05006105006106</v>
       </c>
       <c r="I5" s="1">
-        <v>40969</v>
+        <v>40983</v>
       </c>
       <c r="N5">
         <f>R5*1000/P5</f>
@@ -800,7 +816,7 @@
         <v>154.25315425315426</v>
       </c>
       <c r="I6" s="1">
-        <v>42339</v>
+        <v>42353</v>
       </c>
       <c r="N6">
         <f>R6*1000/P6</f>
@@ -834,7 +850,7 @@
         <v>23</v>
       </c>
       <c r="I7" s="1">
-        <v>36039</v>
+        <v>36053</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -846,7 +862,7 @@
         <v>23</v>
       </c>
       <c r="I8" s="1">
-        <v>40299</v>
+        <v>40313</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -860,13 +876,13 @@
         <v>48</v>
       </c>
       <c r="D9" s="1">
-        <v>38231</v>
+        <v>38245</v>
       </c>
       <c r="E9" s="1">
-        <v>42979</v>
+        <v>42993</v>
       </c>
       <c r="F9" s="1">
-        <v>42795</v>
+        <v>42809</v>
       </c>
       <c r="G9" t="s">
         <v>33</v>
@@ -876,7 +892,7 @@
         <v>454.98750000000001</v>
       </c>
       <c r="I9" s="1">
-        <v>38200</v>
+        <v>38214</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -896,7 +912,7 @@
         <v>33</v>
       </c>
       <c r="I10" s="1">
-        <v>41609</v>
+        <v>41623</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -910,7 +926,7 @@
         <v>1528</v>
       </c>
       <c r="E11" s="1">
-        <v>40603</v>
+        <v>40617</v>
       </c>
       <c r="G11" t="s">
         <v>33</v>
@@ -920,7 +936,7 @@
         <v>5.2722513089005236</v>
       </c>
       <c r="I11" s="1">
-        <v>38200</v>
+        <v>38214</v>
       </c>
       <c r="K11" t="s">
         <v>31</v>
@@ -937,7 +953,7 @@
         <v>1528</v>
       </c>
       <c r="E12" s="1">
-        <v>41883</v>
+        <v>41897</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" t="s">
@@ -948,7 +964,7 @@
         <v>6.0600785340314127</v>
       </c>
       <c r="I12" s="1">
-        <v>40513</v>
+        <v>40527</v>
       </c>
       <c r="K12" t="s">
         <v>31</v>
@@ -965,7 +981,7 @@
         <v>1528</v>
       </c>
       <c r="E13" s="1">
-        <v>42248</v>
+        <v>42262</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" t="s">
@@ -976,14 +992,62 @@
         <v>6.2198298429319365</v>
       </c>
       <c r="I13" s="1">
-        <v>41609</v>
+        <v>41623</v>
       </c>
       <c r="K13" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="G14" s="8"/>
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="9">
+        <v>38944</v>
+      </c>
+      <c r="F14" s="9">
+        <v>38306</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" s="8">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="9">
+        <v>38397</v>
+      </c>
+      <c r="F15" s="9">
+        <v>38306</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" s="8">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="9">
+        <v>38944</v>
+      </c>
+      <c r="F16" s="9">
+        <v>38306</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I16" s="1">
+        <v>2004</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>